<commit_message>
id draft mark added
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A2614A-BD8B-4F94-ACDF-D367CF0EE2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D951152B-9032-4837-BA6D-836E946DD516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="259">
   <si>
     <t>Форпик</t>
   </si>
@@ -617,12 +617,6 @@
     <t>Fr</t>
   </si>
   <si>
-    <t>Осадка на кормовых марках углубления</t>
-  </si>
-  <si>
-    <t>Осадка на носовых марках углубления</t>
-  </si>
-  <si>
     <t>Статический угол крена судна                                    </t>
   </si>
   <si>
@@ -738,6 +732,93 @@
   </si>
   <si>
     <t>Остойчивость</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 80  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на кормовых марках ЛБ                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> м            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 81  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на кормовых марках осредненная                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 82  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на промежуточных кормовых марках ПрБ                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 83  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на промежуточных кормовых марках ЛБ                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 84  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на промежуточных кормовых марках осредненная             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 85  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на миделевых марках ПрБ                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 86  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на миделевых марках ЛБ                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 87  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на миделевых марках осредненная                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 88  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на промежуточных носовых марках ПрБ                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 89  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на промежуточных носовых марках ЛБ                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 90  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на промежуточных носовых марках осредненная              </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 91  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на носовых марках ПрБ                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 92  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на носовых марках ЛБ                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 93  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Осадка на носовых марках осредненная                            </t>
   </si>
 </sst>
 </file>
@@ -1224,15 +1305,15 @@
         <v>78</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2796,7 +2877,7 @@
         <v>164</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D2" s="12">
         <v>7.6189999999999998</v>
@@ -2819,7 +2900,7 @@
         <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D3" s="12">
         <v>5.1710000000000003</v>
@@ -2842,7 +2923,7 @@
         <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D4" s="12">
         <v>6.2E-2</v>
@@ -2865,7 +2946,7 @@
         <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>54</v>
@@ -2888,7 +2969,7 @@
         <v>171</v>
       </c>
       <c r="C6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D6" s="12">
         <v>0.123</v>
@@ -2911,7 +2992,7 @@
         <v>172</v>
       </c>
       <c r="C7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D7" s="12">
         <v>0.06</v>
@@ -2934,7 +3015,7 @@
         <v>173</v>
       </c>
       <c r="C8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D8" s="12">
         <v>0.504</v>
@@ -2957,7 +3038,7 @@
         <v>174</v>
       </c>
       <c r="C9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>54</v>
@@ -2980,7 +3061,7 @@
         <v>175</v>
       </c>
       <c r="C10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>54</v>
@@ -3003,7 +3084,7 @@
         <v>176</v>
       </c>
       <c r="C11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D11" s="12">
         <v>51.542000000000002</v>
@@ -3026,7 +3107,7 @@
         <v>177</v>
       </c>
       <c r="C12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>54</v>
@@ -3049,7 +3130,7 @@
         <v>178</v>
       </c>
       <c r="C13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D13" s="12">
         <v>0.309</v>
@@ -3095,7 +3176,7 @@
         <v>180</v>
       </c>
       <c r="C15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>54</v>
@@ -3118,7 +3199,7 @@
         <v>181</v>
       </c>
       <c r="C16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>54</v>
@@ -3141,7 +3222,7 @@
         <v>182</v>
       </c>
       <c r="C17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>54</v>
@@ -3164,7 +3245,7 @@
         <v>183</v>
       </c>
       <c r="C18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D18" s="12">
         <v>0.2346</v>
@@ -3186,10 +3267,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3197,6 +3278,8 @@
     <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3215,7 +3298,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -3226,10 +3309,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D3" s="12">
         <v>14194.5</v>
@@ -3240,7 +3323,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>157</v>
@@ -3254,7 +3337,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>157</v>
@@ -3268,10 +3351,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D6" s="12">
         <v>6.4329999999999998</v>
@@ -3282,7 +3365,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>157</v>
@@ -3307,7 +3390,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -3318,7 +3401,7 @@
         <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>157</v>
@@ -3332,7 +3415,7 @@
         <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>157</v>
@@ -3346,7 +3429,7 @@
         <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>157</v>
@@ -3360,10 +3443,10 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>54</v>
@@ -3374,10 +3457,10 @@
         <v>89</v>
       </c>
       <c r="B14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D14" s="12">
         <v>-0.03</v>
@@ -3388,7 +3471,7 @@
         <v>152</v>
       </c>
       <c r="B15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>157</v>
@@ -3399,58 +3482,70 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>230</v>
+      </c>
       <c r="B16" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D16" s="12">
+        <v>232</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="B17" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D18" s="12">
         <v>8.6509999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>192</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D17" s="12">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>90</v>
+        <v>237</v>
       </c>
       <c r="B19" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="D19" s="12">
-        <v>19.905000000000001</v>
+        <v>232</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>91</v>
+        <v>239</v>
       </c>
       <c r="B20" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>54</v>
@@ -3458,409 +3553,405 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>92</v>
+        <v>241</v>
       </c>
       <c r="B21" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="D21" s="12">
-        <v>194.232</v>
+        <v>232</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>93</v>
+        <v>243</v>
       </c>
       <c r="B22" t="s">
-        <v>215</v>
+        <v>244</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D22" s="12">
-        <v>4.194</v>
+        <v>232</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>216</v>
+        <v>245</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>246</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D23" s="12">
-        <v>2.72</v>
+        <v>232</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
-        <v>14</v>
+      <c r="A24" s="12" t="s">
+        <v>247</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>248</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D24" s="12">
-        <f>D23+D22</f>
-        <v>6.9139999999999997</v>
+        <v>232</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="B25" t="s">
+        <v>250</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="B26" t="s">
+        <v>252</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B27" t="s">
+        <v>254</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="B28" t="s">
+        <v>256</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D28" s="12">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B29" t="s">
+        <v>258</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" t="s">
+        <v>210</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" s="12">
+        <v>19.905000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" t="s">
+        <v>211</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
+        <v>212</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D33" s="12">
+        <v>194.232</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D34" s="12">
+        <v>4.194</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="12">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36" s="12">
+        <f>D35+D34</f>
+        <v>6.9139999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B37" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D37" s="12">
         <v>0.48099999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
         <v>16</v>
       </c>
-      <c r="B26" t="s">
-        <v>219</v>
-      </c>
-      <c r="C26" s="12" t="s">
+      <c r="B38" t="s">
+        <v>217</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D38" s="13">
         <f>(108.1+17.1+10.8+14.9+101.8)/14194.1</f>
         <v>1.7803171740370997E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
+      <c r="L38" s="12"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
         <v>17</v>
       </c>
-      <c r="B27" t="s">
-        <v>220</v>
-      </c>
-      <c r="C27" s="12" t="s">
+      <c r="B39" t="s">
+        <v>218</v>
+      </c>
+      <c r="C39" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D39" s="13">
         <f>2188.9/14194.1</f>
         <v>0.15421196130786735</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B40" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D40" s="12">
         <v>0.309</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B41" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C41" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D41" s="12">
         <v>178.57599999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B42" t="s">
         <v>107</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C42" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D30" s="12">
-        <f>D29+D22</f>
+      <c r="D42" s="12">
+        <f>D41+D34</f>
         <v>182.76999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B43" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C43" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+      <c r="D43" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B44" t="s">
         <v>111</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C44" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D32" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
+      <c r="D44" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B45" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C45" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D33" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+      <c r="D45" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B46" t="s">
         <v>115</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C46" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D34" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="D46" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B47" t="s">
         <v>117</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+      <c r="C47" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B48" t="s">
         <v>119</v>
       </c>
-      <c r="C36" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="D36" s="12">
+      <c r="C48" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D48" s="12">
         <v>872.72799999999995</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B37" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B38" t="s">
-        <v>123</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="B39" t="s">
-        <v>125</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B40" t="s">
-        <v>127</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D40" s="12">
-        <v>5.1710000000000003</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B41" t="s">
-        <v>129</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D41" s="12">
-        <v>7.47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B42" t="s">
-        <v>131</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B43" t="s">
-        <v>133</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D43" s="12">
-        <v>16.13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="B44" t="s">
-        <v>135</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="D44" s="12">
-        <v>20.608000000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B45" t="s">
-        <v>137</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="D45" s="12">
-        <v>1.771E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B46" t="s">
-        <v>139</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="D46" s="12">
-        <v>0.13492999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="B47" t="s">
-        <v>141</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D47" s="12">
-        <v>25.909099999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B48" t="s">
-        <v>143</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D48" s="12">
-        <v>45.65</v>
-      </c>
+      <c r="L48" s="12"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="B49" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>198</v>
+        <v>157</v>
       </c>
       <c r="D49" s="12" t="s">
         <v>54</v>
@@ -3868,13 +3959,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="B50" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>206</v>
+        <v>157</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>54</v>
@@ -3882,13 +3973,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="B51" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>198</v>
+        <v>157</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>54</v>
@@ -3896,57 +3987,225 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B52" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D52" s="12">
+        <v>5.1710000000000003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D53" s="12">
+        <v>7.47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D55" s="12">
+        <v>16.13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D56" s="12">
+        <v>20.608000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D57" s="12">
+        <v>1.771E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" t="s">
+        <v>139</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D58" s="12">
+        <v>0.13492999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59" s="12">
+        <v>25.909099999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B60" t="s">
+        <v>143</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" s="12">
+        <v>45.65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61" t="s">
+        <v>145</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B63" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B64" t="s">
         <v>151</v>
       </c>
-      <c r="C52" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="12">
+      <c r="C64" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="12">
         <v>53</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B65" t="s">
         <v>160</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C65" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D53" s="12">
+      <c r="D65" s="12">
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="12">
-        <v>54</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="12">
+        <v>54</v>
+      </c>
+      <c r="B66" t="s">
         <v>158</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C66" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D54" s="12">
+      <c r="D66" s="12">
         <v>61.231000000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="12">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="12">
         <v>55</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B67" t="s">
         <v>159</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C67" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D55" s="12">
+      <c r="D67" s="12">
         <v>63.344999999999999</v>
       </c>
     </row>
@@ -3954,7 +4213,7 @@
   <mergeCells count="3">
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
id draft mark fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D951152B-9032-4837-BA6D-836E946DD516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C963939-952E-4158-88A6-552B9C6A27D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3269,8 +3269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3505,8 +3505,8 @@
       <c r="C17" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>54</v>
+      <c r="D17" s="12">
+        <v>8.6509999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3519,8 +3519,8 @@
       <c r="C18" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="D18" s="12">
-        <v>8.6509999999999998</v>
+      <c r="D18" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3659,8 +3659,8 @@
       <c r="C28" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="D28" s="12">
-        <v>7.3</v>
+      <c r="D28" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3673,8 +3673,8 @@
       <c r="C29" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>54</v>
+      <c r="D29" s="12">
+        <v>7.3</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sofia | test 1 | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9F109B-C525-4A38-98D5-487109A1F6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8294F561-7AAB-4E5D-8431-AA9C6B40B6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -2102,7 +2102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD512CFD-1E2E-4C9F-AF20-D54F57AEF969}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -3271,8 +3271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3409,7 +3409,7 @@
         <v>157</v>
       </c>
       <c r="D10" s="12">
-        <v>8.0530000000000008</v>
+        <v>8.0380000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sofia | test1 | tank msfx type added
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8294F561-7AAB-4E5D-8431-AA9C6B40B6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390B84CE-FB0E-4664-8F9F-B1E3AD21556E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10665" yWindow="1230" windowWidth="21600" windowHeight="11385" tabRatio="903" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="262">
   <si>
     <t>Форпик</t>
   </si>
@@ -819,6 +819,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Осадка на носовых марках осредненная                            </t>
+  </si>
+  <si>
+    <t>m_f_s_x type</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -912,7 +921,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -952,6 +961,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1336,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D23"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,7 +1358,8 @@
     <col min="2" max="2" width="45.125" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.375" style="2" customWidth="1"/>
     <col min="4" max="4" width="7.75" style="3"/>
-    <col min="5" max="7" width="7.75" style="2"/>
+    <col min="5" max="5" width="14.75" style="2" customWidth="1"/>
+    <col min="6" max="7" width="7.75" style="2"/>
     <col min="8" max="16384" width="7.75" style="1"/>
   </cols>
   <sheetData>
@@ -1363,7 +1376,9 @@
       <c r="D1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>259</v>
+      </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
@@ -1380,6 +1395,9 @@
       <c r="D2" s="8">
         <v>0</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -1394,6 +1412,9 @@
       <c r="D3" s="8">
         <v>0</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -1408,6 +1429,9 @@
       <c r="D4" s="8">
         <v>0</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -1422,6 +1446,9 @@
       <c r="D5" s="8">
         <v>71.400000000000006</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -1436,6 +1463,9 @@
       <c r="D6" s="8">
         <v>240.2</v>
       </c>
+      <c r="E6" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -1450,6 +1480,9 @@
       <c r="D7" s="8">
         <v>129.80000000000001</v>
       </c>
+      <c r="E7" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1464,6 +1497,9 @@
       <c r="D8" s="8">
         <v>0</v>
       </c>
+      <c r="E8" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -1478,6 +1514,9 @@
       <c r="D9" s="8">
         <v>0</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -1492,6 +1531,9 @@
       <c r="D10" s="8">
         <v>0</v>
       </c>
+      <c r="E10" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -1506,6 +1548,9 @@
       <c r="D11" s="8">
         <v>128.4</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -1520,6 +1565,9 @@
       <c r="D12" s="8">
         <v>0</v>
       </c>
+      <c r="E12" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -1534,6 +1582,9 @@
       <c r="D13" s="8">
         <v>109.3</v>
       </c>
+      <c r="E13" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -1548,6 +1599,9 @@
       <c r="D14" s="8">
         <v>87.1</v>
       </c>
+      <c r="E14" s="2" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1562,6 +1616,9 @@
       <c r="D15" s="8">
         <v>104</v>
       </c>
+      <c r="E15" s="2" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -1576,8 +1633,11 @@
       <c r="D16" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>222</v>
       </c>
@@ -1590,8 +1650,11 @@
       <c r="D17" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>223</v>
       </c>
@@ -1604,8 +1667,11 @@
       <c r="D18" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>224</v>
       </c>
@@ -1618,8 +1684,11 @@
       <c r="D19" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>225</v>
       </c>
@@ -1632,8 +1701,11 @@
       <c r="D20" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>226</v>
       </c>
@@ -1646,8 +1718,11 @@
       <c r="D21" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>227</v>
       </c>
@@ -1660,8 +1735,11 @@
       <c r="D22" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>228</v>
       </c>
@@ -1674,8 +1752,11 @@
       <c r="D23" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>303</v>
       </c>
@@ -1688,8 +1769,11 @@
       <c r="D24" s="8">
         <v>107.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>304</v>
       </c>
@@ -1702,8 +1786,11 @@
       <c r="D25" s="8">
         <v>107.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>305</v>
       </c>
@@ -1716,8 +1803,11 @@
       <c r="D26" s="8">
         <v>77.8</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>306</v>
       </c>
@@ -1730,8 +1820,11 @@
       <c r="D27" s="8">
         <v>99.6</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>229</v>
       </c>
@@ -1744,8 +1837,11 @@
       <c r="D28" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>230</v>
       </c>
@@ -1758,8 +1854,11 @@
       <c r="D29" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>231</v>
       </c>
@@ -1772,8 +1871,11 @@
       <c r="D30" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>232</v>
       </c>
@@ -1786,8 +1888,11 @@
       <c r="D31" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>301</v>
       </c>
@@ -1800,8 +1905,11 @@
       <c r="D32" s="8">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>302</v>
       </c>
@@ -1814,8 +1922,11 @@
       <c r="D33" s="8">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>307</v>
       </c>
@@ -1828,8 +1939,11 @@
       <c r="D34" s="8">
         <v>11.3</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>400</v>
       </c>
@@ -1842,8 +1956,11 @@
       <c r="D35" s="8">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>401</v>
       </c>
@@ -1856,8 +1973,11 @@
       <c r="D36" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>402</v>
       </c>
@@ -1870,8 +1990,11 @@
       <c r="D37" s="8">
         <v>29.9</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>403</v>
       </c>
@@ -1884,8 +2007,11 @@
       <c r="D38" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>501</v>
       </c>
@@ -1898,8 +2024,11 @@
       <c r="D39" s="8">
         <v>17.100000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>502</v>
       </c>
@@ -1909,11 +2038,14 @@
       <c r="C40" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>503</v>
       </c>
@@ -1926,8 +2058,11 @@
       <c r="D41" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>504</v>
       </c>
@@ -1940,8 +2075,11 @@
       <c r="D42" s="8">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>308</v>
       </c>
@@ -1954,8 +2092,11 @@
       <c r="D43" s="8">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>700</v>
       </c>
@@ -1968,8 +2109,11 @@
       <c r="D44" s="8">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>701</v>
       </c>
@@ -1982,8 +2126,11 @@
       <c r="D45" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>702</v>
       </c>
@@ -1996,8 +2143,11 @@
       <c r="D46" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>703</v>
       </c>
@@ -2010,8 +2160,11 @@
       <c r="D47" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>704</v>
       </c>
@@ -2024,8 +2177,11 @@
       <c r="D48" s="8">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>705</v>
       </c>
@@ -2038,8 +2194,11 @@
       <c r="D49" s="8">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>706</v>
       </c>
@@ -2052,8 +2211,11 @@
       <c r="D50" s="8">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>601</v>
       </c>
@@ -2066,8 +2228,11 @@
       <c r="D51" s="8">
         <v>36.299999999999997</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>602</v>
       </c>
@@ -2080,19 +2245,34 @@
       <c r="D52" s="8">
         <v>36.299999999999997</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>991</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="8"/>
+      <c r="C53" s="9">
+        <v>0</v>
+      </c>
+      <c r="D53" s="8">
+        <v>0</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>260</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E53" xr:uid="{85F60F57-DBE3-404F-8261-7C9C9497D4F6}">
+      <formula1>"max,current"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -2103,7 +2283,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3271,7 +3451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sofia | test | added
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9F2691-CDA8-4573-9C97-9116D27B7762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BC56C3-CE7C-44FC-AB85-E25A6724225F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -975,11 +975,11 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1301,7 +1301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1C353A-23EF-4F36-B9F8-6A3A925A383A}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -1355,7 +1355,7 @@
       <c r="A6" t="s">
         <v>263</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>265</v>
       </c>
     </row>
@@ -3058,7 +3058,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3462,7 +3462,7 @@
         <v>219</v>
       </c>
       <c r="D18" s="12">
-        <v>0.2346</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E18" t="s">
         <v>166</v>
@@ -3483,8 +3483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3511,12 +3511,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -3603,12 +3603,12 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -3892,12 +3892,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
@@ -4009,8 +4009,8 @@
         <v>157</v>
       </c>
       <c r="D38" s="13">
-        <f>(108.1+17.1+10.8+14.9+101.8)/14194.1</f>
-        <v>1.7803171740370997E-2</v>
+        <f>(108.1+17.1+10.8+14.9+101.8)/D3</f>
+        <v>1.7802670048258126E-2</v>
       </c>
       <c r="L38" s="12"/>
     </row>
@@ -4025,8 +4025,8 @@
         <v>157</v>
       </c>
       <c r="D39" s="13">
-        <f>2188.9/14194.1</f>
-        <v>0.15421196130786735</v>
+        <f>2188.9/D3</f>
+        <v>0.15420761562577054</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sofia | test1 | strength | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BC56C3-CE7C-44FC-AB85-E25A6724225F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA94CD9-E244-4F9C-A827-993349F393AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="262">
   <si>
     <t>Форпик</t>
   </si>
@@ -539,9 +539,6 @@
     <t xml:space="preserve"> Критерий погоды                        </t>
   </si>
   <si>
-    <t xml:space="preserve"> -           </t>
-  </si>
-  <si>
     <t xml:space="preserve">        </t>
   </si>
   <si>
@@ -701,18 +698,6 @@
     <t>Поправка от балласта к поперечной метацентрической высоте</t>
   </si>
   <si>
-    <t xml:space="preserve">м           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">м∙рад       </t>
-  </si>
-  <si>
-    <t>град        </t>
-  </si>
-  <si>
-    <t>м∙град      </t>
-  </si>
-  <si>
     <t>м∙рад</t>
   </si>
   <si>
@@ -840,6 +825,9 @@
   </si>
   <si>
     <t>В соответвствии с "Дополнительные расчеты остойчивости, выполненные в связи с изменением и увеличением осадки. (2020)"</t>
+  </si>
+  <si>
+    <t>м∙град</t>
   </si>
 </sst>
 </file>
@@ -1332,31 +1320,31 @@
         <v>78</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -1409,7 +1397,7 @@
         <v>56</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -1428,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1445,7 +1433,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1462,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1479,7 +1467,7 @@
         <v>71.400000000000006</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1496,7 +1484,7 @@
         <v>240.2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1513,7 +1501,7 @@
         <v>129.80000000000001</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1530,7 +1518,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1547,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1564,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1581,7 +1569,7 @@
         <v>128.4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1598,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1615,7 +1603,7 @@
         <v>109.3</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1632,7 +1620,7 @@
         <v>87.1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1649,7 +1637,7 @@
         <v>104</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1666,7 +1654,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1683,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1700,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1717,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1734,7 +1722,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1751,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1768,7 +1756,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1785,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1802,7 +1790,7 @@
         <v>107.9</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1819,7 +1807,7 @@
         <v>107.9</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1836,7 +1824,7 @@
         <v>77.8</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1853,7 +1841,7 @@
         <v>99.6</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1870,7 +1858,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1887,7 +1875,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1904,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1921,7 +1909,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1938,7 +1926,7 @@
         <v>19.7</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1955,7 +1943,7 @@
         <v>17</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1972,7 +1960,7 @@
         <v>11.3</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1989,7 +1977,7 @@
         <v>5.2</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2006,7 +1994,7 @@
         <v>0.5</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2023,7 +2011,7 @@
         <v>29.9</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2040,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2057,7 +2045,7 @@
         <v>17.100000000000001</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2074,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2091,7 +2079,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2108,7 +2096,7 @@
         <v>3.7</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2125,7 +2113,7 @@
         <v>0.8</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2142,7 +2130,7 @@
         <v>2.7</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2159,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2176,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2193,7 +2181,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2210,7 +2198,7 @@
         <v>0.9</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2227,7 +2215,7 @@
         <v>0.7</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2244,7 +2232,7 @@
         <v>0.7</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2261,7 +2249,7 @@
         <v>36.299999999999997</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2278,7 +2266,7 @@
         <v>36.299999999999997</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2295,7 +2283,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2783,26 +2771,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2769FB-623F-4B71-8DF9-7FDDF69C0946}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>188</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2859,6 +2847,48 @@
       </c>
       <c r="D5" s="12">
         <v>311.10000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>71.739999999999995</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="12">
+        <v>14352.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>13.73</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="12">
+        <v>11739</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="12">
+        <v>1541</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -3058,26 +3088,26 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.25" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C1" t="s">
         <v>184</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>183</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>153</v>
@@ -3090,20 +3120,20 @@
       <c r="B2" t="s">
         <v>164</v>
       </c>
-      <c r="C2" t="s">
-        <v>216</v>
+      <c r="C2" s="12" t="s">
+        <v>215</v>
       </c>
       <c r="D2" s="12">
         <v>7.6189999999999998</v>
       </c>
       <c r="E2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" t="s">
         <v>166</v>
       </c>
-      <c r="F2" t="s">
-        <v>167</v>
-      </c>
       <c r="G2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3111,22 +3141,22 @@
         <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C3" t="s">
-        <v>196</v>
+        <v>167</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="D3" s="12">
         <v>5.1710000000000003</v>
       </c>
       <c r="E3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" t="s">
         <v>166</v>
       </c>
-      <c r="F3" t="s">
-        <v>167</v>
-      </c>
       <c r="G3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3134,22 +3164,22 @@
         <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C4" t="s">
-        <v>223</v>
+        <v>168</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="D4" s="12">
         <v>6.2E-2</v>
       </c>
       <c r="E4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" t="s">
         <v>166</v>
       </c>
-      <c r="F4" t="s">
-        <v>167</v>
-      </c>
       <c r="G4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3157,22 +3187,22 @@
         <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C5" t="s">
-        <v>220</v>
+        <v>169</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" t="s">
         <v>166</v>
       </c>
-      <c r="F5" t="s">
-        <v>167</v>
-      </c>
       <c r="G5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3180,22 +3210,22 @@
         <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C6" t="s">
-        <v>220</v>
+        <v>170</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="D6" s="12">
         <v>0.123</v>
       </c>
       <c r="E6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" t="s">
         <v>166</v>
       </c>
-      <c r="F6" t="s">
-        <v>167</v>
-      </c>
       <c r="G6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3203,22 +3233,22 @@
         <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C7" t="s">
-        <v>220</v>
+        <v>171</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="D7" s="12">
         <v>0.06</v>
       </c>
       <c r="E7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F7" t="s">
         <v>166</v>
       </c>
-      <c r="F7" t="s">
-        <v>167</v>
-      </c>
       <c r="G7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3226,22 +3256,22 @@
         <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C8" t="s">
-        <v>219</v>
+        <v>172</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="D8" s="12">
         <v>0.504</v>
       </c>
       <c r="E8" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" t="s">
         <v>166</v>
       </c>
-      <c r="F8" t="s">
-        <v>167</v>
-      </c>
       <c r="G8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3249,22 +3279,22 @@
         <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>174</v>
-      </c>
-      <c r="C9" t="s">
-        <v>219</v>
+        <v>173</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" t="s">
         <v>166</v>
       </c>
-      <c r="F9" t="s">
-        <v>167</v>
-      </c>
       <c r="G9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3272,22 +3302,22 @@
         <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>175</v>
-      </c>
-      <c r="C10" t="s">
-        <v>219</v>
+        <v>174</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E10" t="s">
+        <v>165</v>
+      </c>
+      <c r="F10" t="s">
         <v>166</v>
       </c>
-      <c r="F10" t="s">
-        <v>167</v>
-      </c>
       <c r="G10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3295,22 +3325,22 @@
         <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" t="s">
-        <v>221</v>
+        <v>175</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="D11" s="12">
         <v>51.542000000000002</v>
       </c>
       <c r="E11" t="s">
+        <v>165</v>
+      </c>
+      <c r="F11" t="s">
         <v>166</v>
       </c>
-      <c r="F11" t="s">
-        <v>167</v>
-      </c>
       <c r="G11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3318,22 +3348,22 @@
         <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" t="s">
-        <v>221</v>
+        <v>176</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" t="s">
         <v>166</v>
       </c>
-      <c r="F12" t="s">
-        <v>167</v>
-      </c>
       <c r="G12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3341,22 +3371,22 @@
         <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>178</v>
-      </c>
-      <c r="C13" t="s">
-        <v>219</v>
+        <v>177</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="D13" s="12">
         <v>0.309</v>
       </c>
       <c r="E13" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" t="s">
         <v>166</v>
       </c>
-      <c r="F13" t="s">
-        <v>167</v>
-      </c>
       <c r="G13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3364,22 +3394,22 @@
         <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>179</v>
-      </c>
-      <c r="C14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" t="s">
         <v>165</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>166</v>
       </c>
-      <c r="F14" t="s">
-        <v>167</v>
-      </c>
       <c r="G14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3387,22 +3417,22 @@
         <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C15" t="s">
-        <v>221</v>
+        <v>179</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E15" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" t="s">
         <v>166</v>
       </c>
-      <c r="F15" t="s">
-        <v>167</v>
-      </c>
       <c r="G15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3410,22 +3440,22 @@
         <v>98</v>
       </c>
       <c r="B16" t="s">
-        <v>181</v>
-      </c>
-      <c r="C16" t="s">
-        <v>221</v>
+        <v>180</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E16" t="s">
+        <v>165</v>
+      </c>
+      <c r="F16" t="s">
         <v>166</v>
       </c>
-      <c r="F16" t="s">
-        <v>167</v>
-      </c>
       <c r="G16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3433,22 +3463,22 @@
         <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>182</v>
-      </c>
-      <c r="C17" t="s">
-        <v>222</v>
+        <v>181</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>261</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E17" t="s">
+        <v>165</v>
+      </c>
+      <c r="F17" t="s">
         <v>166</v>
       </c>
-      <c r="F17" t="s">
-        <v>167</v>
-      </c>
       <c r="G17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3456,22 +3486,22 @@
         <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>183</v>
-      </c>
-      <c r="C18" t="s">
-        <v>219</v>
+        <v>182</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="D18" s="12">
         <v>0.28000000000000003</v>
       </c>
       <c r="E18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" t="s">
         <v>166</v>
       </c>
-      <c r="F18" t="s">
-        <v>167</v>
-      </c>
       <c r="G18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3483,7 +3513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -3512,7 +3542,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -3523,10 +3553,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D3" s="12">
         <v>14194.5</v>
@@ -3537,7 +3567,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>157</v>
@@ -3551,7 +3581,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>157</v>
@@ -3565,10 +3595,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D6" s="12">
         <v>6.4329999999999998</v>
@@ -3579,7 +3609,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>157</v>
@@ -3604,7 +3634,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -3615,7 +3645,7 @@
         <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>157</v>
@@ -3629,7 +3659,7 @@
         <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>157</v>
@@ -3643,7 +3673,7 @@
         <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>157</v>
@@ -3657,10 +3687,10 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>54</v>
@@ -3671,10 +3701,10 @@
         <v>89</v>
       </c>
       <c r="B14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D14" s="12">
         <v>-0.03</v>
@@ -3685,7 +3715,7 @@
         <v>152</v>
       </c>
       <c r="B15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>157</v>
@@ -3697,13 +3727,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B16" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>54</v>
@@ -3711,13 +3741,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B17" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D17" s="12">
         <v>8.6509999999999998</v>
@@ -3725,13 +3755,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B18" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>54</v>
@@ -3739,13 +3769,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B19" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>54</v>
@@ -3753,13 +3783,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B20" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>54</v>
@@ -3767,13 +3797,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B21" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>54</v>
@@ -3781,13 +3811,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B22" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>54</v>
@@ -3795,13 +3825,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B23" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D23" s="12">
         <v>7.9960000000000004</v>
@@ -3809,13 +3839,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B24" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>54</v>
@@ -3823,13 +3853,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B25" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>54</v>
@@ -3837,13 +3867,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B26" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>54</v>
@@ -3851,13 +3881,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B27" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>54</v>
@@ -3865,13 +3895,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B28" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>54</v>
@@ -3879,13 +3909,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B29" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D29" s="12">
         <v>7.3</v>
@@ -3893,7 +3923,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -3904,10 +3934,10 @@
         <v>90</v>
       </c>
       <c r="B31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D31" s="12">
         <v>19.905000000000001</v>
@@ -3918,10 +3948,10 @@
         <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>54</v>
@@ -3932,10 +3962,10 @@
         <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D33" s="12">
         <v>194.232</v>
@@ -3946,7 +3976,7 @@
         <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>157</v>
@@ -3957,7 +3987,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B35" t="s">
         <v>96</v>
@@ -4003,7 +4033,7 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>157</v>
@@ -4019,7 +4049,7 @@
         <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>157</v>
@@ -4136,7 +4166,7 @@
         <v>117</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>54</v>
@@ -4150,7 +4180,7 @@
         <v>119</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D48" s="12">
         <v>872.72799999999995</v>
@@ -4207,7 +4237,7 @@
         <v>127</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D52" s="12">
         <v>5.1710000000000003</v>
@@ -4221,7 +4251,7 @@
         <v>129</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D53" s="12">
         <v>7.47</v>
@@ -4235,7 +4265,7 @@
         <v>131</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>54</v>
@@ -4249,7 +4279,7 @@
         <v>133</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D55" s="12">
         <v>16.13</v>
@@ -4263,7 +4293,7 @@
         <v>135</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D56" s="12">
         <v>20.608000000000001</v>
@@ -4277,7 +4307,7 @@
         <v>137</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D57" s="12">
         <v>1.771E-2</v>
@@ -4291,7 +4321,7 @@
         <v>139</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D58" s="12">
         <v>0.13492999999999999</v>
@@ -4305,7 +4335,7 @@
         <v>141</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D59" s="12">
         <v>25.909099999999999</v>
@@ -4319,7 +4349,7 @@
         <v>143</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D60" s="12">
         <v>45.65</v>
@@ -4333,7 +4363,7 @@
         <v>145</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D61" s="12" t="s">
         <v>54</v>
@@ -4347,7 +4377,7 @@
         <v>147</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D62" s="12" t="s">
         <v>54</v>
@@ -4361,7 +4391,7 @@
         <v>149</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D63" s="12" t="s">
         <v>54</v>
@@ -4375,7 +4405,7 @@
         <v>151</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
sofia | test | error added
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA94CD9-E244-4F9C-A827-993349F393AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1327F6-13D8-4310-8CCA-5C7CF58A5025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -23,6 +23,9 @@
     <sheet name="StabilityCriteria" sheetId="62" r:id="rId8"/>
     <sheet name="Parameters" sheetId="65" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="Max">Parameters!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="264">
   <si>
     <t>Форпик</t>
   </si>
@@ -620,9 +623,6 @@
     <t xml:space="preserve">Осадка на кормовом перпендикуляре                               </t>
   </si>
   <si>
-    <t>Осадка средняя                                                  </t>
-  </si>
-  <si>
     <t>Осадка на носовом перпендикуляре                                </t>
   </si>
   <si>
@@ -635,9 +635,6 @@
     <t>т</t>
   </si>
   <si>
-    <t xml:space="preserve">м </t>
-  </si>
-  <si>
     <t>Абсцисса центра тяжести</t>
   </si>
   <si>
@@ -725,9 +722,6 @@
     <t xml:space="preserve"> Осадка на кормовых марках ЛБ                                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> м            </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 81  </t>
   </si>
   <si>
@@ -828,6 +822,21 @@
   </si>
   <si>
     <t>м∙град</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> м</t>
+  </si>
+  <si>
+    <t>Погрешность относительная</t>
+  </si>
+  <si>
+    <t>Погрешность абсолютная</t>
+  </si>
+  <si>
+    <t>Осадка в цт площади ватерлинии                                                 </t>
+  </si>
+  <si>
+    <t>±0,5 % ширины судна</t>
   </si>
 </sst>
 </file>
@@ -921,7 +930,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -968,6 +977,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1290,7 +1308,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1320,36 +1338,36 @@
         <v>78</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9 B3" xr:uid="{237807A0-C7C0-4C70-AA77-B5C8A04904F8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8 B3" xr:uid="{237807A0-C7C0-4C70-AA77-B5C8A04904F8}">
       <formula1>"none,full,half"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{F3A3F7AF-522E-4FA1-9E89-6D2966A02B38}">
@@ -1368,7 +1386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
@@ -1397,7 +1415,7 @@
         <v>56</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -1416,7 +1434,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1433,7 +1451,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1450,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1467,7 +1485,7 @@
         <v>71.400000000000006</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1484,7 +1502,7 @@
         <v>240.2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1501,7 +1519,7 @@
         <v>129.80000000000001</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1518,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1535,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1552,7 +1570,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1569,7 +1587,7 @@
         <v>128.4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1586,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1603,7 +1621,7 @@
         <v>109.3</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1620,7 +1638,7 @@
         <v>87.1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1637,7 +1655,7 @@
         <v>104</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1654,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1671,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1688,7 +1706,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1705,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1722,7 +1740,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1739,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1756,7 +1774,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1773,7 +1791,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1790,7 +1808,7 @@
         <v>107.9</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,7 +1825,7 @@
         <v>107.9</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1824,7 +1842,7 @@
         <v>77.8</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1841,7 +1859,7 @@
         <v>99.6</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1858,7 +1876,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1875,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1892,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1909,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1926,7 +1944,7 @@
         <v>19.7</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1943,7 +1961,7 @@
         <v>17</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1960,7 +1978,7 @@
         <v>11.3</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1977,7 +1995,7 @@
         <v>5.2</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1994,7 +2012,7 @@
         <v>0.5</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2011,7 +2029,7 @@
         <v>29.9</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2028,7 +2046,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2045,7 +2063,7 @@
         <v>17.100000000000001</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2062,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2079,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2096,7 +2114,7 @@
         <v>3.7</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2113,7 +2131,7 @@
         <v>0.8</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2130,7 +2148,7 @@
         <v>2.7</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2147,7 +2165,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2164,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2181,7 +2199,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2198,7 +2216,7 @@
         <v>0.9</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2215,7 +2233,7 @@
         <v>0.7</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2232,7 +2250,7 @@
         <v>0.7</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2249,7 +2267,7 @@
         <v>36.299999999999997</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2266,7 +2284,7 @@
         <v>36.299999999999997</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2283,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -2771,29 +2789,39 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2769FB-623F-4B71-8DF9-7FDDF69C0946}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
+    <col min="6" max="6" width="15.125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="17" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>18.600000000000001</v>
       </c>
@@ -2806,8 +2834,14 @@
       <c r="D2" s="12">
         <v>6973.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="12">
+        <v>5</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>39.32</v>
       </c>
@@ -2820,8 +2854,14 @@
       <c r="D3" s="12">
         <v>-4251.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="12">
+        <v>5</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>91.12</v>
       </c>
@@ -2834,8 +2874,14 @@
       <c r="D4" s="12">
         <v>1088.0999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="12">
+        <v>5</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>119.98</v>
       </c>
@@ -2848,8 +2894,14 @@
       <c r="D5" s="12">
         <v>311.10000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="12">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>71.739999999999995</v>
       </c>
@@ -2862,8 +2914,14 @@
       <c r="D6" s="12">
         <v>14352.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="12">
+        <v>5</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>13.73</v>
       </c>
@@ -2876,8 +2934,14 @@
       <c r="D7" s="12">
         <v>11739</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="12">
+        <v>5</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>18.600000000000001</v>
       </c>
@@ -2890,6 +2954,15 @@
       <c r="D8" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="E8" s="12">
+        <v>5</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2898,184 +2971,312 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5DE354-6FE8-4F4E-92DF-8FA9F59E1489}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.375" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="17" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>-40</v>
       </c>
       <c r="B2" s="12">
         <v>-0.41739999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="12">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>-35</v>
       </c>
       <c r="B3" s="12">
         <v>-0.34689999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="12">
+        <v>5</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>-30</v>
       </c>
       <c r="B4" s="12">
         <v>-0.2752</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="12">
+        <v>5</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>-25</v>
       </c>
       <c r="B5" s="12">
         <v>-0.2228</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="12">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>-20</v>
       </c>
       <c r="B6" s="12">
         <v>-0.1628</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="12">
+        <v>5</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>-15</v>
       </c>
       <c r="B7" s="12">
         <v>-0.105</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="12">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>-10</v>
       </c>
       <c r="B8" s="12">
         <v>-6.25E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="12">
+        <v>5</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>-5</v>
       </c>
       <c r="B9" s="12">
         <v>-2.87E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="12">
+        <v>5</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>0</v>
       </c>
       <c r="B10" s="12">
         <v>-1E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="12">
+        <v>5</v>
+      </c>
+      <c r="D10" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>5</v>
       </c>
       <c r="B11" s="12">
         <v>2.8400000000000002E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="12">
+        <v>5</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>10</v>
       </c>
       <c r="B12" s="12">
         <v>6.2199999999999998E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>15</v>
       </c>
       <c r="B13" s="12">
         <v>0.1047</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="12">
+        <v>5</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>20</v>
       </c>
       <c r="B14" s="12">
         <v>0.16259999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="12">
+        <v>5</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>25</v>
       </c>
       <c r="B15" s="12">
         <v>0.2225</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="12">
+        <v>5</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>30</v>
       </c>
       <c r="B16" s="12">
         <v>0.27489999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="12">
+        <v>5</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>35</v>
       </c>
       <c r="B17" s="12">
         <v>0.34660000000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="12">
+        <v>5</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>40</v>
       </c>
       <c r="B18" s="12">
         <v>0.41720000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="12">
+        <v>5</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>45</v>
       </c>
       <c r="B19" s="12">
         <v>0.47210000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="12">
+        <v>5</v>
+      </c>
+      <c r="D19" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>50</v>
       </c>
       <c r="B20" s="12">
         <v>0.50239999999999996</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="12">
+        <v>5</v>
+      </c>
+      <c r="D20" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>55</v>
       </c>
       <c r="B21" s="12">
         <v>0.49490000000000001</v>
+      </c>
+      <c r="C21" s="12">
+        <v>5</v>
+      </c>
+      <c r="D21" s="12">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -3088,7 +3289,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3097,20 +3298,28 @@
     <col min="2" max="2" width="41.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.875" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.25" customWidth="1"/>
+    <col min="6" max="6" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="17" t="s">
         <v>153</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3121,16 +3330,16 @@
         <v>164</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D2" s="12">
         <v>7.6189999999999998</v>
       </c>
-      <c r="E2" t="s">
-        <v>165</v>
-      </c>
-      <c r="F2" t="s">
-        <v>166</v>
+      <c r="E2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="G2" t="s">
         <v>165</v>
@@ -3144,16 +3353,16 @@
         <v>167</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D3" s="12">
         <v>5.1710000000000003</v>
       </c>
-      <c r="E3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F3" t="s">
-        <v>166</v>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="G3" t="s">
         <v>165</v>
@@ -3167,16 +3376,16 @@
         <v>168</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D4" s="12">
         <v>6.2E-2</v>
       </c>
-      <c r="E4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F4" t="s">
-        <v>166</v>
+      <c r="E4" s="12">
+        <v>5</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="G4" t="s">
         <v>165</v>
@@ -3190,16 +3399,16 @@
         <v>169</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F5" t="s">
-        <v>166</v>
+      <c r="E5" s="12">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="G5" t="s">
         <v>165</v>
@@ -3213,16 +3422,16 @@
         <v>170</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D6" s="12">
         <v>0.123</v>
       </c>
-      <c r="E6" t="s">
-        <v>165</v>
-      </c>
-      <c r="F6" t="s">
-        <v>166</v>
+      <c r="E6" s="12">
+        <v>5</v>
+      </c>
+      <c r="F6" s="12">
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="G6" t="s">
         <v>165</v>
@@ -3236,16 +3445,16 @@
         <v>171</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D7" s="12">
         <v>0.06</v>
       </c>
-      <c r="E7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F7" t="s">
-        <v>166</v>
+      <c r="E7" s="12">
+        <v>5</v>
+      </c>
+      <c r="F7" s="12">
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="G7" t="s">
         <v>165</v>
@@ -3264,11 +3473,11 @@
       <c r="D8" s="12">
         <v>0.504</v>
       </c>
-      <c r="E8" t="s">
-        <v>165</v>
-      </c>
-      <c r="F8" t="s">
-        <v>166</v>
+      <c r="E8" s="12">
+        <v>5</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0.05</v>
       </c>
       <c r="G8" t="s">
         <v>165</v>
@@ -3287,11 +3496,11 @@
       <c r="D9" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E9" t="s">
-        <v>165</v>
-      </c>
-      <c r="F9" t="s">
-        <v>166</v>
+      <c r="E9" s="12">
+        <v>5</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0.05</v>
       </c>
       <c r="G9" t="s">
         <v>165</v>
@@ -3310,11 +3519,11 @@
       <c r="D10" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E10" t="s">
-        <v>165</v>
-      </c>
-      <c r="F10" t="s">
-        <v>166</v>
+      <c r="E10" s="12">
+        <v>5</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0.05</v>
       </c>
       <c r="G10" t="s">
         <v>165</v>
@@ -3328,16 +3537,16 @@
         <v>175</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D11" s="12">
         <v>51.542000000000002</v>
       </c>
-      <c r="E11" t="s">
-        <v>165</v>
-      </c>
-      <c r="F11" t="s">
-        <v>166</v>
+      <c r="E11" s="12">
+        <v>1</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="G11" t="s">
         <v>165</v>
@@ -3351,16 +3560,16 @@
         <v>176</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E12" t="s">
-        <v>165</v>
-      </c>
-      <c r="F12" t="s">
-        <v>166</v>
+      <c r="E12" s="12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="G12" t="s">
         <v>165</v>
@@ -3379,11 +3588,11 @@
       <c r="D13" s="12">
         <v>0.309</v>
       </c>
-      <c r="E13" t="s">
-        <v>165</v>
-      </c>
-      <c r="F13" t="s">
-        <v>166</v>
+      <c r="E13" s="12">
+        <v>1</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0.05</v>
       </c>
       <c r="G13" t="s">
         <v>165</v>
@@ -3397,16 +3606,16 @@
         <v>178</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E14" t="s">
-        <v>165</v>
-      </c>
-      <c r="F14" t="s">
-        <v>166</v>
+      <c r="E14" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="G14" t="s">
         <v>165</v>
@@ -3420,15 +3629,15 @@
         <v>179</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E15" t="s">
-        <v>165</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E15" s="12">
+        <v>1</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>166</v>
       </c>
       <c r="G15" t="s">
@@ -3443,15 +3652,15 @@
         <v>180</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E16" t="s">
-        <v>165</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E16" s="12">
+        <v>1</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>166</v>
       </c>
       <c r="G16" t="s">
@@ -3466,16 +3675,16 @@
         <v>181</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E17" t="s">
-        <v>165</v>
-      </c>
-      <c r="F17" t="s">
-        <v>166</v>
+      <c r="E17" s="12">
+        <v>5</v>
+      </c>
+      <c r="F17" s="12">
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="G17" t="s">
         <v>165</v>
@@ -3494,11 +3703,11 @@
       <c r="D18" s="12">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F18" t="s">
-        <v>166</v>
+      <c r="E18" s="12">
+        <v>1</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0.05</v>
       </c>
       <c r="G18" t="s">
         <v>165</v>
@@ -3513,61 +3722,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="21.875" customWidth="1"/>
+    <col min="6" max="6" width="19.125" customWidth="1"/>
     <col min="9" max="9" width="4.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="17" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D3" s="12">
         <v>14194.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="12">
+        <v>2</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>157</v>
@@ -3575,13 +3800,19 @@
       <c r="D4" s="12">
         <v>63.371000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>157</v>
@@ -3589,27 +3820,39 @@
       <c r="D5" s="12">
         <v>63.371000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>197</v>
+        <v>157</v>
       </c>
       <c r="D6" s="12">
         <v>6.4329999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>157</v>
@@ -3617,8 +3860,14 @@
       <c r="D7" s="12">
         <v>6.6050000000000004</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>52</v>
       </c>
@@ -3631,21 +3880,29 @@
       <c r="D8" s="12">
         <v>-1E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>192</v>
+        <v>262</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>157</v>
@@ -3653,13 +3910,19 @@
       <c r="D10" s="12">
         <v>8.0380000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>157</v>
@@ -3667,8 +3930,14 @@
       <c r="D11" s="12">
         <v>7.2889999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="12">
+        <v>1</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>87</v>
       </c>
@@ -3681,22 +3950,34 @@
       <c r="D12" s="12">
         <v>8.7029999999999994</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>89</v>
       </c>
@@ -3704,18 +3985,24 @@
         <v>190</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D14" s="12">
         <v>-0.03</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>152</v>
       </c>
       <c r="B15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>157</v>
@@ -3724,236 +4011,340 @@
         <f>D11-D12</f>
         <v>-1.4139999999999997</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="12">
+        <v>1</v>
+      </c>
+      <c r="F15" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B16" t="s">
+        <v>224</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="12">
+        <v>1</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>226</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="B17" t="s">
-        <v>229</v>
-      </c>
       <c r="C17" s="12" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="D17" s="12">
         <v>8.6509999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="12">
+        <v>1</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="B18" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B19" t="s">
         <v>230</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C19" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1</v>
+      </c>
+      <c r="F19" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="B20" t="s">
         <v>232</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C20" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="12">
+        <v>1</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="B21" t="s">
         <v>234</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C21" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="12">
+        <v>1</v>
+      </c>
+      <c r="F21" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="B22" t="s">
         <v>236</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C22" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="12">
+        <v>1</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="B23" t="s">
         <v>238</v>
       </c>
-      <c r="B22" t="s">
-        <v>239</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="B23" t="s">
-        <v>241</v>
-      </c>
       <c r="C23" s="12" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="D23" s="12">
         <v>7.9960000000000004</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="12">
+        <v>1</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B24" t="s">
+        <v>240</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="12">
+        <v>1</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B25" t="s">
         <v>242</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C25" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="B26" t="s">
         <v>244</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C26" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="12">
+        <v>1</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="B27" t="s">
         <v>246</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C27" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="12">
+        <v>1</v>
+      </c>
+      <c r="F27" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="B28" t="s">
         <v>248</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C28" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="12">
+        <v>1</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="B29" t="s">
         <v>250</v>
       </c>
-      <c r="B28" t="s">
-        <v>251</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="B29" t="s">
-        <v>253</v>
-      </c>
       <c r="C29" s="12" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="D29" s="12">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="12">
+        <v>1</v>
+      </c>
+      <c r="F29" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>90</v>
       </c>
       <c r="B31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D31" s="12">
         <v>19.905000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D32" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3962,13 +4353,19 @@
         <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D33" s="12">
         <v>194.232</v>
+      </c>
+      <c r="E33" s="12">
+        <v>2</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -3976,7 +4373,7 @@
         <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>157</v>
@@ -3984,10 +4381,16 @@
       <c r="D34" s="12">
         <v>4.194</v>
       </c>
+      <c r="E34" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
         <v>96</v>
@@ -3997,6 +4400,12 @@
       </c>
       <c r="D35" s="12">
         <v>2.72</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -4013,6 +4422,12 @@
         <f>D35+D34</f>
         <v>6.9139999999999997</v>
       </c>
+      <c r="E36" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
@@ -4027,13 +4442,19 @@
       <c r="D37" s="12">
         <v>0.48099999999999998</v>
       </c>
+      <c r="E37" s="12">
+        <v>1</v>
+      </c>
+      <c r="F37" s="12">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>157</v>
@@ -4042,6 +4463,12 @@
         <f>(108.1+17.1+10.8+14.9+101.8)/D3</f>
         <v>1.7802670048258126E-2</v>
       </c>
+      <c r="E38" s="12">
+        <v>2</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="L38" s="12"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -4049,7 +4476,7 @@
         <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>157</v>
@@ -4058,6 +4485,12 @@
         <f>2188.9/D3</f>
         <v>0.15420761562577054</v>
       </c>
+      <c r="E39" s="12">
+        <v>2</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
@@ -4072,6 +4505,12 @@
       <c r="D40" s="12">
         <v>0.309</v>
       </c>
+      <c r="E40" s="12">
+        <v>1</v>
+      </c>
+      <c r="F40" s="12">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
@@ -4086,6 +4525,12 @@
       <c r="D41" s="12">
         <v>178.57599999999999</v>
       </c>
+      <c r="E41" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
@@ -4101,6 +4546,12 @@
         <f>D41+D34</f>
         <v>182.76999999999998</v>
       </c>
+      <c r="E42" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
@@ -4115,6 +4566,12 @@
       <c r="D43" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="E43" s="12">
+        <v>1</v>
+      </c>
+      <c r="F43" s="12">
+        <v>50</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
@@ -4129,6 +4586,12 @@
       <c r="D44" s="13" t="s">
         <v>54</v>
       </c>
+      <c r="E44" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
@@ -4143,6 +4606,12 @@
       <c r="D45" s="13" t="s">
         <v>54</v>
       </c>
+      <c r="E45" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
@@ -4157,6 +4626,12 @@
       <c r="D46" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="E46" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
@@ -4166,9 +4641,15 @@
         <v>117</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D47" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F47" s="12" t="s">
         <v>54</v>
       </c>
     </row>
@@ -4180,14 +4661,20 @@
         <v>119</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D48" s="12">
         <v>872.72799999999995</v>
       </c>
+      <c r="E48" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="L48" s="12"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>120</v>
       </c>
@@ -4200,8 +4687,14 @@
       <c r="D49" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="12">
+        <v>5</v>
+      </c>
+      <c r="F49" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>122</v>
       </c>
@@ -4214,8 +4707,14 @@
       <c r="D50" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="12">
+        <v>5</v>
+      </c>
+      <c r="F50" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>124</v>
       </c>
@@ -4228,8 +4727,14 @@
       <c r="D51" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="12">
+        <v>5</v>
+      </c>
+      <c r="F51" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>126</v>
       </c>
@@ -4237,13 +4742,19 @@
         <v>127</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D52" s="12">
         <v>5.1710000000000003</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F52" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>128</v>
       </c>
@@ -4251,13 +4762,19 @@
         <v>129</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D53" s="12">
         <v>7.47</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F53" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>130</v>
       </c>
@@ -4265,13 +4782,19 @@
         <v>131</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F54" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>132</v>
       </c>
@@ -4279,13 +4802,19 @@
         <v>133</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D55" s="12">
         <v>16.13</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F55" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>134</v>
       </c>
@@ -4293,13 +4822,19 @@
         <v>135</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D56" s="12">
         <v>20.608000000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>136</v>
       </c>
@@ -4307,13 +4842,19 @@
         <v>137</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D57" s="12">
         <v>1.771E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>138</v>
       </c>
@@ -4321,13 +4862,19 @@
         <v>139</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D58" s="12">
         <v>0.13492999999999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>140</v>
       </c>
@@ -4335,13 +4882,19 @@
         <v>141</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D59" s="12">
         <v>25.909099999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F59" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>142</v>
       </c>
@@ -4349,13 +4902,19 @@
         <v>143</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D60" s="12">
         <v>45.65</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F60" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>144</v>
       </c>
@@ -4363,13 +4922,19 @@
         <v>145</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D61" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F61" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>146</v>
       </c>
@@ -4377,13 +4942,19 @@
         <v>147</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D62" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="12">
+        <v>5</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>148</v>
       </c>
@@ -4391,13 +4962,19 @@
         <v>149</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D63" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F63" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>150</v>
       </c>
@@ -4405,13 +4982,19 @@
         <v>151</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="12">
         <v>53</v>
       </c>
@@ -4424,8 +5007,14 @@
       <c r="D65" s="12">
         <v>-1E-3</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F65" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="12">
         <v>54</v>
       </c>
@@ -4438,8 +5027,14 @@
       <c r="D66" s="12">
         <v>61.231000000000002</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="12">
+        <v>1</v>
+      </c>
+      <c r="F66" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="12">
         <v>55</v>
       </c>
@@ -4452,12 +5047,18 @@
       <c r="D67" s="12">
         <v>63.344999999999999</v>
       </c>
+      <c r="E67" s="12">
+        <v>1</v>
+      </c>
+      <c r="F67" s="12">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
sofia | test| BM&SF | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1327F6-13D8-4310-8CCA-5C7CF58A5025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DBE77A-8C28-44BE-934E-BFF0176C54DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -19,9 +19,10 @@
     <sheet name="GrainBulkheads" sheetId="55" r:id="rId4"/>
     <sheet name="Stores" sheetId="57" r:id="rId5"/>
     <sheet name="SF&amp;BM" sheetId="63" r:id="rId6"/>
-    <sheet name="Stabilitycurve" sheetId="61" r:id="rId7"/>
-    <sheet name="StabilityCriteria" sheetId="62" r:id="rId8"/>
-    <sheet name="Parameters" sheetId="65" r:id="rId9"/>
+    <sheet name="SF&amp;BM_max" sheetId="66" r:id="rId7"/>
+    <sheet name="Stabilitycurve" sheetId="61" r:id="rId8"/>
+    <sheet name="StabilityCriteria" sheetId="62" r:id="rId9"/>
+    <sheet name="Parameters" sheetId="65" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="Max">Parameters!#REF!</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="269">
   <si>
     <t>Форпик</t>
   </si>
@@ -837,6 +838,21 @@
   </si>
   <si>
     <t>±0,5 % ширины судна</t>
+  </si>
+  <si>
+    <t>BMmax_abs</t>
+  </si>
+  <si>
+    <t>BMmax_perc</t>
+  </si>
+  <si>
+    <t>SFmax_abs</t>
+  </si>
+  <si>
+    <t>SFmax_perc</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -975,9 +991,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -986,6 +999,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1382,6 +1398,1353 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
+  <dimension ref="A1:L67"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="21.875" customWidth="1"/>
+    <col min="6" max="6" width="19.125" customWidth="1"/>
+    <col min="9" max="9" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="60" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="12">
+        <v>14194.5</v>
+      </c>
+      <c r="E3" s="12">
+        <v>2</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="12">
+        <v>63.371000000000002</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="12">
+        <v>63.371000000000002</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="12">
+        <v>6.4329999999999998</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="12">
+        <v>6.6050000000000004</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="12">
+        <v>-1E-3</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" s="12">
+        <v>8.0380000000000003</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="12">
+        <v>7.2889999999999997</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="12">
+        <v>8.7029999999999994</v>
+      </c>
+      <c r="E12" s="12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D14" s="12">
+        <v>-0.03</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="12">
+        <f>D11-D12</f>
+        <v>-1.4139999999999997</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1</v>
+      </c>
+      <c r="F15" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B16" t="s">
+        <v>224</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="12">
+        <v>1</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B17" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D17" s="12">
+        <v>8.6509999999999998</v>
+      </c>
+      <c r="E17" s="12">
+        <v>1</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="B18" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B19" t="s">
+        <v>230</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1</v>
+      </c>
+      <c r="F19" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B20" t="s">
+        <v>232</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="12">
+        <v>1</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21" t="s">
+        <v>234</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="12">
+        <v>1</v>
+      </c>
+      <c r="F21" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="12">
+        <v>1</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B23" t="s">
+        <v>238</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D23" s="12">
+        <v>7.9960000000000004</v>
+      </c>
+      <c r="E23" s="12">
+        <v>1</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B24" t="s">
+        <v>240</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="12">
+        <v>1</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B25" t="s">
+        <v>242</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B26" t="s">
+        <v>244</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="12">
+        <v>1</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="B27" t="s">
+        <v>246</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="12">
+        <v>1</v>
+      </c>
+      <c r="F27" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B28" t="s">
+        <v>248</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="12">
+        <v>1</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="B29" t="s">
+        <v>250</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D29" s="12">
+        <v>7.3</v>
+      </c>
+      <c r="E29" s="12">
+        <v>1</v>
+      </c>
+      <c r="F29" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" t="s">
+        <v>207</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D31" s="12">
+        <v>19.905000000000001</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D33" s="12">
+        <v>194.232</v>
+      </c>
+      <c r="E33" s="12">
+        <v>2</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" t="s">
+        <v>210</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D34" s="12">
+        <v>4.194</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="12">
+        <v>2.72</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36" s="12">
+        <f>D35+D34</f>
+        <v>6.9139999999999997</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" s="12">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="E37" s="12">
+        <v>1</v>
+      </c>
+      <c r="F37" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
+        <v>16</v>
+      </c>
+      <c r="B38" t="s">
+        <v>214</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38" s="13">
+        <f>(108.1+17.1+10.8+14.9+101.8)/D3</f>
+        <v>1.7802670048258126E-2</v>
+      </c>
+      <c r="E38" s="12">
+        <v>2</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="L38" s="12"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
+        <v>17</v>
+      </c>
+      <c r="B39" t="s">
+        <v>215</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" s="13">
+        <f>2188.9/D3</f>
+        <v>0.15420761562577054</v>
+      </c>
+      <c r="E39" s="12">
+        <v>2</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="12">
+        <v>0.309</v>
+      </c>
+      <c r="E40" s="12">
+        <v>1</v>
+      </c>
+      <c r="F40" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" s="12">
+        <v>178.57599999999999</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42" s="12">
+        <f>D41+D34</f>
+        <v>182.76999999999998</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" s="12">
+        <v>1</v>
+      </c>
+      <c r="F43" s="12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D48" s="12">
+        <v>872.72799999999995</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="L48" s="12"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49" s="12">
+        <v>5</v>
+      </c>
+      <c r="F49" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E50" s="12">
+        <v>5</v>
+      </c>
+      <c r="F50" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" t="s">
+        <v>125</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E51" s="12">
+        <v>5</v>
+      </c>
+      <c r="F51" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B52" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D52" s="12">
+        <v>5.1710000000000003</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F52" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D53" s="12">
+        <v>7.47</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F53" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F54" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D55" s="12">
+        <v>16.13</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F55" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D56" s="12">
+        <v>20.608000000000001</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D57" s="12">
+        <v>1.771E-2</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" t="s">
+        <v>139</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D58" s="12">
+        <v>0.13492999999999999</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D59" s="12">
+        <v>25.909099999999999</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F59" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B60" t="s">
+        <v>143</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D60" s="12">
+        <v>45.65</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F60" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61" t="s">
+        <v>145</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F61" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E62" s="12">
+        <v>5</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B63" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F63" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B64" t="s">
+        <v>151</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="12">
+        <v>53</v>
+      </c>
+      <c r="B65" t="s">
+        <v>160</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D65" s="12">
+        <v>-1E-3</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F65" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="12">
+        <v>54</v>
+      </c>
+      <c r="B66" t="s">
+        <v>158</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D66" s="12">
+        <v>61.231000000000002</v>
+      </c>
+      <c r="E66" s="12">
+        <v>1</v>
+      </c>
+      <c r="F66" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="12">
+        <v>55</v>
+      </c>
+      <c r="B67" t="s">
+        <v>159</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D67" s="12">
+        <v>63.344999999999999</v>
+      </c>
+      <c r="E67" s="12">
+        <v>1</v>
+      </c>
+      <c r="F67" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A9:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G53"/>
@@ -2789,10 +4152,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2769FB-623F-4B71-8DF9-7FDDF69C0946}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2801,23 +4164,23 @@
     <col min="6" max="6" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:6" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>261</v>
       </c>
     </row>
@@ -2900,69 +4263,6 @@
       <c r="F5" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
-        <v>71.739999999999995</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="12">
-        <v>14352.2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>5</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
-        <v>13.73</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="12">
-        <v>11739</v>
-      </c>
-      <c r="E7" s="12">
-        <v>5</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="12">
-        <v>1541</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="12">
-        <v>5</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F9" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2970,6 +4270,112 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C060607D-3FA9-4A65-9257-6535830146B9}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="5" max="5" width="15.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="12">
+        <v>71.739999999999995</v>
+      </c>
+      <c r="C2" s="12">
+        <v>14352.2</v>
+      </c>
+      <c r="D2" s="12">
+        <v>5</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="12">
+        <v>13.73</v>
+      </c>
+      <c r="C3" s="12">
+        <v>11739</v>
+      </c>
+      <c r="D3" s="12">
+        <v>5</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B4" s="12">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="C4" s="12">
+        <v>-1541</v>
+      </c>
+      <c r="D4" s="12">
+        <v>5</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B5" s="12">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="C5" s="12">
+        <v>-1541</v>
+      </c>
+      <c r="D5" s="12">
+        <v>5</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5DE354-6FE8-4F4E-92DF-8FA9F59E1489}">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -2986,16 +4392,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>261</v>
       </c>
     </row>
@@ -3284,7 +4690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E500720D-7F16-4373-97E5-9F957C7E1B58}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -3303,22 +4709,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>261</v>
       </c>
     </row>
@@ -3716,1351 +5122,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
-  <dimension ref="A1:L67"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="5" max="5" width="21.875" customWidth="1"/>
-    <col min="6" max="6" width="19.125" customWidth="1"/>
-    <col min="9" max="9" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="60" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D3" s="12">
-        <v>14194.5</v>
-      </c>
-      <c r="E3" s="12">
-        <v>2</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D4" s="12">
-        <v>63.371000000000002</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>56</v>
-      </c>
-      <c r="B5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" s="12">
-        <v>63.371000000000002</v>
-      </c>
-      <c r="E5" s="12">
-        <v>1</v>
-      </c>
-      <c r="F5" s="12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D6" s="12">
-        <v>6.4329999999999998</v>
-      </c>
-      <c r="E6" s="12">
-        <v>1</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>199</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" s="12">
-        <v>6.6050000000000004</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>52</v>
-      </c>
-      <c r="B8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D8" s="12">
-        <v>-1E-3</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="F8" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" t="s">
-        <v>262</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D10" s="12">
-        <v>8.0380000000000003</v>
-      </c>
-      <c r="E10" s="12">
-        <v>1</v>
-      </c>
-      <c r="F10" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" t="s">
-        <v>192</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="12">
-        <v>7.2889999999999997</v>
-      </c>
-      <c r="E11" s="12">
-        <v>1</v>
-      </c>
-      <c r="F11" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D12" s="12">
-        <v>8.7029999999999994</v>
-      </c>
-      <c r="E12" s="12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>212</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" t="s">
-        <v>190</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D14" s="12">
-        <v>-0.03</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" t="s">
-        <v>193</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D15" s="12">
-        <f>D11-D12</f>
-        <v>-1.4139999999999997</v>
-      </c>
-      <c r="E15" s="12">
-        <v>1</v>
-      </c>
-      <c r="F15" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="B16" t="s">
-        <v>224</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="12">
-        <v>1</v>
-      </c>
-      <c r="F16" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="B17" t="s">
-        <v>226</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D17" s="12">
-        <v>8.6509999999999998</v>
-      </c>
-      <c r="E17" s="12">
-        <v>1</v>
-      </c>
-      <c r="F17" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="B18" t="s">
-        <v>228</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="12">
-        <v>1</v>
-      </c>
-      <c r="F18" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="B19" t="s">
-        <v>230</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="12">
-        <v>1</v>
-      </c>
-      <c r="F19" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="B20" t="s">
-        <v>232</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="12">
-        <v>1</v>
-      </c>
-      <c r="F20" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="B21" t="s">
-        <v>234</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="12">
-        <v>1</v>
-      </c>
-      <c r="F21" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="B22" t="s">
-        <v>236</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="12">
-        <v>1</v>
-      </c>
-      <c r="F22" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="B23" t="s">
-        <v>238</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D23" s="12">
-        <v>7.9960000000000004</v>
-      </c>
-      <c r="E23" s="12">
-        <v>1</v>
-      </c>
-      <c r="F23" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="B24" t="s">
-        <v>240</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="12">
-        <v>1</v>
-      </c>
-      <c r="F24" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="B25" t="s">
-        <v>242</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="12">
-        <v>1</v>
-      </c>
-      <c r="F25" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="B26" t="s">
-        <v>244</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="12">
-        <v>1</v>
-      </c>
-      <c r="F26" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="B27" t="s">
-        <v>246</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="12">
-        <v>1</v>
-      </c>
-      <c r="F27" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="B28" t="s">
-        <v>248</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="12">
-        <v>1</v>
-      </c>
-      <c r="F28" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="B29" t="s">
-        <v>250</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D29" s="12">
-        <v>7.3</v>
-      </c>
-      <c r="E29" s="12">
-        <v>1</v>
-      </c>
-      <c r="F29" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" t="s">
-        <v>207</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D31" s="12">
-        <v>19.905000000000001</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" t="s">
-        <v>208</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" t="s">
-        <v>209</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="D33" s="12">
-        <v>194.232</v>
-      </c>
-      <c r="E33" s="12">
-        <v>2</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B34" t="s">
-        <v>210</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D34" s="12">
-        <v>4.194</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="B35" t="s">
-        <v>96</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D35" s="12">
-        <v>2.72</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="12">
-        <v>14</v>
-      </c>
-      <c r="B36" t="s">
-        <v>161</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D36" s="12">
-        <f>D35+D34</f>
-        <v>6.9139999999999997</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B37" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D37" s="12">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="E37" s="12">
-        <v>1</v>
-      </c>
-      <c r="F37" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="12">
-        <v>16</v>
-      </c>
-      <c r="B38" t="s">
-        <v>214</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D38" s="13">
-        <f>(108.1+17.1+10.8+14.9+101.8)/D3</f>
-        <v>1.7802670048258126E-2</v>
-      </c>
-      <c r="E38" s="12">
-        <v>2</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="L38" s="12"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="12">
-        <v>17</v>
-      </c>
-      <c r="B39" t="s">
-        <v>215</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D39" s="13">
-        <f>2188.9/D3</f>
-        <v>0.15420761562577054</v>
-      </c>
-      <c r="E39" s="12">
-        <v>2</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D40" s="12">
-        <v>0.309</v>
-      </c>
-      <c r="E40" s="12">
-        <v>1</v>
-      </c>
-      <c r="F40" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B41" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D41" s="12">
-        <v>178.57599999999999</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B42" t="s">
-        <v>107</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D42" s="12">
-        <f>D41+D34</f>
-        <v>182.76999999999998</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B43" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E43" s="12">
-        <v>1</v>
-      </c>
-      <c r="F43" s="12">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B44" t="s">
-        <v>111</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B45" t="s">
-        <v>113</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B46" t="s">
-        <v>115</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F46" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B47" t="s">
-        <v>117</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B48" t="s">
-        <v>119</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="D48" s="12">
-        <v>872.72799999999995</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="L48" s="12"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B49" t="s">
-        <v>121</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E49" s="12">
-        <v>5</v>
-      </c>
-      <c r="F49" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B50" t="s">
-        <v>123</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E50" s="12">
-        <v>5</v>
-      </c>
-      <c r="F50" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="B51" t="s">
-        <v>125</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E51" s="12">
-        <v>5</v>
-      </c>
-      <c r="F51" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B52" t="s">
-        <v>127</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D52" s="12">
-        <v>5.1710000000000003</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F52" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B53" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D53" s="12">
-        <v>7.47</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F53" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B54" t="s">
-        <v>131</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F54" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B55" t="s">
-        <v>133</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D55" s="12">
-        <v>16.13</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F55" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="B56" t="s">
-        <v>135</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="D56" s="12">
-        <v>20.608000000000001</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F56" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B57" t="s">
-        <v>137</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="D57" s="12">
-        <v>1.771E-2</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B58" t="s">
-        <v>139</v>
-      </c>
-      <c r="C58" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="D58" s="12">
-        <v>0.13492999999999999</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F58" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="B59" t="s">
-        <v>141</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D59" s="12">
-        <v>25.909099999999999</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F59" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B60" t="s">
-        <v>143</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D60" s="12">
-        <v>45.65</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F60" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="B61" t="s">
-        <v>145</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F61" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B62" t="s">
-        <v>147</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E62" s="12">
-        <v>5</v>
-      </c>
-      <c r="F62" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="B63" t="s">
-        <v>149</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F63" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="B64" t="s">
-        <v>151</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F64" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="12">
-        <v>53</v>
-      </c>
-      <c r="B65" t="s">
-        <v>160</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D65" s="12">
-        <v>-1E-3</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="F65" s="12">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="12">
-        <v>54</v>
-      </c>
-      <c r="B66" t="s">
-        <v>158</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D66" s="12">
-        <v>61.231000000000002</v>
-      </c>
-      <c r="E66" s="12">
-        <v>1</v>
-      </c>
-      <c r="F66" s="12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="12">
-        <v>55</v>
-      </c>
-      <c r="B67" t="s">
-        <v>159</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D67" s="12">
-        <v>63.344999999999999</v>
-      </c>
-      <c r="E67" s="12">
-        <v>1</v>
-      </c>
-      <c r="F67" s="12">
-        <v>0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A9:F9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
test | error | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DBE77A-8C28-44BE-934E-BFF0176C54DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF39F29-977A-44C0-8F04-E213F67CEBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -1402,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2250,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="12">
-        <v>50</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -4273,7 +4273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C060607D-3FA9-4A65-9257-6535830146B9}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sofia | test1 | error | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF39F29-977A-44C0-8F04-E213F67CEBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D3A116-F9DC-46ED-99C2-0319AFB49ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="268">
   <si>
     <t>Форпик</t>
   </si>
@@ -544,9 +544,6 @@
   </si>
   <si>
     <t xml:space="preserve">        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     </t>
   </si>
   <si>
     <t xml:space="preserve"> Статический крен от ветра              </t>
@@ -1354,31 +1351,31 @@
         <v>78</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -1402,7 +1399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
@@ -1431,15 +1428,15 @@
         <v>153</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>260</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -1452,10 +1449,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D3" s="12">
         <v>14194.5</v>
@@ -1472,7 +1469,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>157</v>
@@ -1492,7 +1489,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>157</v>
@@ -1512,7 +1509,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>157</v>
@@ -1532,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>157</v>
@@ -1561,7 +1558,7 @@
         <v>-1E-3</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F8" s="12">
         <v>0.05</v>
@@ -1569,7 +1566,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -1582,7 +1579,7 @@
         <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>157</v>
@@ -1602,7 +1599,7 @@
         <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>157</v>
@@ -1622,7 +1619,7 @@
         <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>157</v>
@@ -1642,10 +1639,10 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>54</v>
@@ -1662,10 +1659,10 @@
         <v>89</v>
       </c>
       <c r="B14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D14" s="12">
         <v>-0.03</v>
@@ -1682,7 +1679,7 @@
         <v>152</v>
       </c>
       <c r="B15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>157</v>
@@ -1700,13 +1697,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B16" t="s">
         <v>223</v>
       </c>
-      <c r="B16" t="s">
-        <v>224</v>
-      </c>
       <c r="C16" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>54</v>
@@ -1720,13 +1717,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="B17" t="s">
         <v>225</v>
       </c>
-      <c r="B17" t="s">
-        <v>226</v>
-      </c>
       <c r="C17" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D17" s="12">
         <v>8.6509999999999998</v>
@@ -1740,13 +1737,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B18" t="s">
         <v>227</v>
       </c>
-      <c r="B18" t="s">
-        <v>228</v>
-      </c>
       <c r="C18" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>54</v>
@@ -1760,13 +1757,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="B19" t="s">
         <v>229</v>
       </c>
-      <c r="B19" t="s">
-        <v>230</v>
-      </c>
       <c r="C19" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>54</v>
@@ -1780,13 +1777,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B20" t="s">
         <v>231</v>
       </c>
-      <c r="B20" t="s">
-        <v>232</v>
-      </c>
       <c r="C20" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>54</v>
@@ -1800,13 +1797,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B21" t="s">
         <v>233</v>
       </c>
-      <c r="B21" t="s">
-        <v>234</v>
-      </c>
       <c r="C21" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>54</v>
@@ -1820,13 +1817,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="B22" t="s">
         <v>235</v>
       </c>
-      <c r="B22" t="s">
-        <v>236</v>
-      </c>
       <c r="C22" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>54</v>
@@ -1840,13 +1837,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="B23" t="s">
         <v>237</v>
       </c>
-      <c r="B23" t="s">
-        <v>238</v>
-      </c>
       <c r="C23" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D23" s="12">
         <v>7.9960000000000004</v>
@@ -1860,13 +1857,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B24" t="s">
         <v>239</v>
       </c>
-      <c r="B24" t="s">
-        <v>240</v>
-      </c>
       <c r="C24" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>54</v>
@@ -1880,13 +1877,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B25" t="s">
         <v>241</v>
       </c>
-      <c r="B25" t="s">
-        <v>242</v>
-      </c>
       <c r="C25" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>54</v>
@@ -1900,13 +1897,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B26" t="s">
         <v>243</v>
       </c>
-      <c r="B26" t="s">
-        <v>244</v>
-      </c>
       <c r="C26" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>54</v>
@@ -1920,13 +1917,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B27" t="s">
         <v>245</v>
       </c>
-      <c r="B27" t="s">
-        <v>246</v>
-      </c>
       <c r="C27" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>54</v>
@@ -1940,13 +1937,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="B28" t="s">
         <v>247</v>
       </c>
-      <c r="B28" t="s">
-        <v>248</v>
-      </c>
       <c r="C28" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>54</v>
@@ -1960,13 +1957,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B29" t="s">
         <v>249</v>
       </c>
-      <c r="B29" t="s">
-        <v>250</v>
-      </c>
       <c r="C29" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D29" s="12">
         <v>7.3</v>
@@ -1980,7 +1977,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -1993,10 +1990,10 @@
         <v>90</v>
       </c>
       <c r="B31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D31" s="12">
         <v>19.905000000000001</v>
@@ -2013,10 +2010,10 @@
         <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>54</v>
@@ -2033,10 +2030,10 @@
         <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D33" s="12">
         <v>194.232</v>
@@ -2053,7 +2050,7 @@
         <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>157</v>
@@ -2070,7 +2067,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B35" t="s">
         <v>96</v>
@@ -2134,7 +2131,7 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>157</v>
@@ -2156,7 +2153,7 @@
         <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>157</v>
@@ -2321,7 +2318,7 @@
         <v>117</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>54</v>
@@ -2341,7 +2338,7 @@
         <v>119</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D48" s="12">
         <v>872.72799999999995</v>
@@ -2422,7 +2419,7 @@
         <v>127</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D52" s="12">
         <v>5.1710000000000003</v>
@@ -2442,7 +2439,7 @@
         <v>129</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D53" s="12">
         <v>7.47</v>
@@ -2462,7 +2459,7 @@
         <v>131</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>54</v>
@@ -2482,7 +2479,7 @@
         <v>133</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D55" s="12">
         <v>16.13</v>
@@ -2502,7 +2499,7 @@
         <v>135</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D56" s="12">
         <v>20.608000000000001</v>
@@ -2522,7 +2519,7 @@
         <v>137</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D57" s="12">
         <v>1.771E-2</v>
@@ -2542,7 +2539,7 @@
         <v>139</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D58" s="12">
         <v>0.13492999999999999</v>
@@ -2562,7 +2559,7 @@
         <v>141</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D59" s="12">
         <v>25.909099999999999</v>
@@ -2582,7 +2579,7 @@
         <v>143</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D60" s="12">
         <v>45.65</v>
@@ -2602,7 +2599,7 @@
         <v>145</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D61" s="12" t="s">
         <v>54</v>
@@ -2622,7 +2619,7 @@
         <v>147</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D62" s="12" t="s">
         <v>54</v>
@@ -2642,7 +2639,7 @@
         <v>149</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D63" s="12" t="s">
         <v>54</v>
@@ -2662,7 +2659,7 @@
         <v>151</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>54</v>
@@ -2688,7 +2685,7 @@
         <v>-1E-3</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F65" s="12">
         <v>0.05</v>
@@ -2778,7 +2775,7 @@
         <v>56</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -2797,7 +2794,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2814,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2831,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2848,7 +2845,7 @@
         <v>71.400000000000006</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2865,7 +2862,7 @@
         <v>240.2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2882,7 +2879,7 @@
         <v>129.80000000000001</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2899,7 +2896,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2916,7 +2913,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2933,7 +2930,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2950,7 +2947,7 @@
         <v>128.4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2967,7 +2964,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2984,7 +2981,7 @@
         <v>109.3</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3001,7 +2998,7 @@
         <v>87.1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3018,7 +3015,7 @@
         <v>104</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3035,7 +3032,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3052,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3069,7 +3066,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3086,7 +3083,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3103,7 +3100,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3120,7 +3117,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3137,7 +3134,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3154,7 +3151,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3171,7 +3168,7 @@
         <v>107.9</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3188,7 +3185,7 @@
         <v>107.9</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3205,7 +3202,7 @@
         <v>77.8</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3222,7 +3219,7 @@
         <v>99.6</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3239,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3256,7 +3253,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3273,7 +3270,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3290,7 +3287,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3307,7 +3304,7 @@
         <v>19.7</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3324,7 +3321,7 @@
         <v>17</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3341,7 +3338,7 @@
         <v>11.3</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3358,7 +3355,7 @@
         <v>5.2</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3375,7 +3372,7 @@
         <v>0.5</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3392,7 +3389,7 @@
         <v>29.9</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3409,7 +3406,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3426,7 +3423,7 @@
         <v>17.100000000000001</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3443,7 +3440,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3460,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3477,7 +3474,7 @@
         <v>3.7</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3494,7 +3491,7 @@
         <v>0.8</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3511,7 +3508,7 @@
         <v>2.7</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3528,7 +3525,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3545,7 +3542,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3562,7 +3559,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3579,7 +3576,7 @@
         <v>0.9</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3596,7 +3593,7 @@
         <v>0.7</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3613,7 +3610,7 @@
         <v>0.7</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3630,7 +3627,7 @@
         <v>36.299999999999997</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3647,7 +3644,7 @@
         <v>36.299999999999997</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3664,7 +3661,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -4166,22 +4163,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>188</v>
-      </c>
       <c r="E1" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>260</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4290,21 +4287,21 @@
         <v>65</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D1" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>260</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B2" s="12">
         <v>71.739999999999995</v>
@@ -4321,7 +4318,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B3" s="12">
         <v>13.73</v>
@@ -4338,7 +4335,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B4" s="12">
         <v>18.600000000000001</v>
@@ -4355,7 +4352,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B5" s="12">
         <v>18.600000000000001</v>
@@ -4399,10 +4396,10 @@
         <v>162</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>260</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4694,8 +4691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E500720D-7F16-4373-97E5-9F957C7E1B58}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4710,22 +4707,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>153</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>260</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4736,7 +4733,7 @@
         <v>164</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D2" s="12">
         <v>7.6189999999999998</v>
@@ -4756,19 +4753,19 @@
         <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D3" s="12">
         <v>5.1710000000000003</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="12">
         <v>1</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="G3" t="s">
         <v>165</v>
@@ -4779,10 +4776,10 @@
         <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D4" s="12">
         <v>6.2E-2</v>
@@ -4802,10 +4799,10 @@
         <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>54</v>
@@ -4825,10 +4822,10 @@
         <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D6" s="12">
         <v>0.123</v>
@@ -4848,10 +4845,10 @@
         <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D7" s="12">
         <v>0.06</v>
@@ -4871,7 +4868,7 @@
         <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>157</v>
@@ -4894,7 +4891,7 @@
         <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>157</v>
@@ -4917,7 +4914,7 @@
         <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>157</v>
@@ -4940,19 +4937,19 @@
         <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D11" s="12">
         <v>51.542000000000002</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="12">
         <v>1</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="G11" t="s">
         <v>165</v>
@@ -4963,19 +4960,19 @@
         <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="12">
         <v>1</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="G12" t="s">
         <v>165</v>
@@ -4986,7 +4983,7 @@
         <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>157</v>
@@ -5009,10 +5006,10 @@
         <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>54</v>
@@ -5032,19 +5029,19 @@
         <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="12">
         <v>1</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>166</v>
       </c>
       <c r="G15" t="s">
         <v>165</v>
@@ -5055,19 +5052,19 @@
         <v>98</v>
       </c>
       <c r="B16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="12">
         <v>1</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>166</v>
       </c>
       <c r="G16" t="s">
         <v>165</v>
@@ -5078,10 +5075,10 @@
         <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>54</v>
@@ -5101,7 +5098,7 @@
         <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>157</v>

</xml_diff>

<commit_message>
parameters correction | added
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D3A116-F9DC-46ED-99C2-0319AFB49ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5BE64A-85DD-4635-A004-EE0AB8BE0B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="269">
   <si>
     <t>Форпик</t>
   </si>
@@ -850,6 +850,9 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>Поправка к поперечной метацентрической высоте</t>
   </si>
 </sst>
 </file>
@@ -1397,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68:F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2729,6 +2732,27 @@
       </c>
       <c r="F67" s="12">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="12">
+        <v>95</v>
+      </c>
+      <c r="B68" t="s">
+        <v>268</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D68" s="13">
+        <f>D38+D39</f>
+        <v>0.17201028567402865</v>
+      </c>
+      <c r="E68" s="12">
+        <v>2</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -4377,7 +4401,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4691,8 +4715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E500720D-7F16-4373-97E5-9F957C7E1B58}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
parameter correction | added
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5BE64A-85DD-4635-A004-EE0AB8BE0B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015D42A1-3AA8-4930-8560-8A725EDC8623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="269">
   <si>
     <t>Форпик</t>
   </si>
@@ -1402,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68:F68"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2143,8 +2143,8 @@
         <f>(108.1+17.1+10.8+14.9+101.8)/D3</f>
         <v>1.7802670048258126E-2</v>
       </c>
-      <c r="E38" s="12">
-        <v>2</v>
+      <c r="E38" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>54</v>
@@ -2165,8 +2165,8 @@
         <f>2188.9/D3</f>
         <v>0.15420761562577054</v>
       </c>
-      <c r="E39" s="12">
-        <v>2</v>
+      <c r="E39" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>54</v>

</xml_diff>